<commit_message>
1. Changed default font from Helvetica to Circe Light 2. Added CSS themes 3. Added possibility to extract parameters of fields from pdf and changed FieldLayouter behaviour 4. Changed ResizeableBorder behaviour to more smooth. 5. Minor changes like adding comments and clearing up code
</commit_message>
<xml_diff>
--- a/src/test/testResources/excels/test.xlsx
+++ b/src/test/testResources/excels/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreyserebryanskiy/IdeaProjects/badgeGenerator/src/test/testResources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreyserebryanskiy/IdeaProjects/badgeGenerator/src/test/testResources/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,40 +32,40 @@
     <t>Фамилия</t>
   </si>
   <si>
+    <t>Андрей</t>
+  </si>
+  <si>
+    <t>Георгиевский</t>
+  </si>
+  <si>
+    <t>Предприниматель</t>
+  </si>
+  <si>
+    <t>Сергей</t>
+  </si>
+  <si>
+    <t>Белобородский</t>
+  </si>
+  <si>
+    <t>Заместитель главы правления по вопросам транспорта</t>
+  </si>
+  <si>
+    <t>Кирилл</t>
+  </si>
+  <si>
+    <t>Беловодов</t>
+  </si>
+  <si>
+    <t>Младший ассистент главного архитектора</t>
+  </si>
+  <si>
+    <t>Максим</t>
+  </si>
+  <si>
+    <t>Сергеев</t>
+  </si>
+  <si>
     <t>Должность</t>
-  </si>
-  <si>
-    <t>Андрей</t>
-  </si>
-  <si>
-    <t>Георгиевский</t>
-  </si>
-  <si>
-    <t>Предприниматель</t>
-  </si>
-  <si>
-    <t>Сергей</t>
-  </si>
-  <si>
-    <t>Белобородский</t>
-  </si>
-  <si>
-    <t>Заместитель главы правления по вопросам транспорта</t>
-  </si>
-  <si>
-    <t>Кирилл</t>
-  </si>
-  <si>
-    <t>Беловодов</t>
-  </si>
-  <si>
-    <t>Младший ассистент главного архитектора</t>
-  </si>
-  <si>
-    <t>Максим</t>
-  </si>
-  <si>
-    <t>Сергеев</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -396,48 +396,48 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>